<commit_message>
Updates on schematic and board layout to hw3_1, optimizations and improvement on layout
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00420B4-3291-4266-AB3C-E6B946AE91AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56743B9C-CCD9-4D87-BC59-902D76FE9F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="251">
   <si>
     <t>References</t>
   </si>
@@ -216,9 +216,6 @@
     <t>771-PMEG6020ER-115</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>Adafruit_240x320_TFT</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>652-SF-2410FP100W-2</t>
   </si>
   <si>
-    <t>S1, S2, S3</t>
-  </si>
-  <si>
     <t>Apem</t>
   </si>
   <si>
@@ -436,9 +430,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Quantity</t>
-  </si>
-  <si>
-    <t>AxxSolder V3.0</t>
   </si>
   <si>
     <t>GCT</t>
@@ -767,6 +758,27 @@
   </si>
   <si>
     <t>R13, R16, R34, R43, R46, R47, R48</t>
+  </si>
+  <si>
+    <t>S2, S3</t>
+  </si>
+  <si>
+    <t>AxxSolder V3.1</t>
+  </si>
+  <si>
+    <t>TFT1</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>TSW-108-07-T-S</t>
+  </si>
+  <si>
+    <t>TSW-108-XX-YY-S</t>
+  </si>
+  <si>
+    <t>200-TSW10807TS</t>
   </si>
 </sst>
 </file>
@@ -922,7 +934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -955,6 +967,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1296,10 +1311,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3ACC24B-AB82-4A13-8EC7-565525F2C562}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,28 +1332,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>213</v>
+      <c r="A1" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>210</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="20"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1359,30 +1374,30 @@
         <v>2</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1416,7 +1431,7 @@
     </row>
     <row r="5" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>9</v>
@@ -1440,17 +1455,17 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="I5" s="13">
-        <f t="shared" ref="I5:I45" si="0">G5*H5</f>
+        <f t="shared" ref="I5:I46" si="0">G5*H5</f>
         <v>2.8319999999999999</v>
       </c>
       <c r="J5" s="13">
-        <f t="shared" ref="J5:J45" si="1">1.25*I5</f>
+        <f t="shared" ref="J5:J46" si="1">1.25*I5</f>
         <v>3.54</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -1465,7 +1480,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -1484,22 +1499,22 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G7" s="11">
         <v>1</v>
@@ -1518,7 +1533,7 @@
     </row>
     <row r="8" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1552,7 +1567,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>20</v>
@@ -1586,7 +1601,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -1620,7 +1635,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>29</v>
@@ -1654,7 +1669,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -1688,7 +1703,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B13" s="11">
         <v>100</v>
@@ -1722,7 +1737,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
@@ -1756,22 +1771,22 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G15" s="11">
         <v>1</v>
@@ -1790,22 +1805,22 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -1827,7 +1842,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>42</v>
@@ -1836,10 +1851,10 @@
         <v>40</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G17" s="11">
         <v>1</v>
@@ -1964,7 +1979,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>58</v>
@@ -1998,22 +2013,22 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="E22" s="1">
         <v>4311</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
@@ -2032,22 +2047,22 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G23" s="11">
         <v>1</v>
@@ -2066,22 +2081,22 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
@@ -2100,22 +2115,22 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G25" s="11">
         <v>1</v>
@@ -2134,22 +2149,22 @@
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G26" s="1">
         <v>1</v>
@@ -2168,44 +2183,44 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>78</v>
+        <v>244</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G27" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27" s="14">
         <v>0.54900000000000004</v>
       </c>
       <c r="I27" s="13">
         <f t="shared" si="0"/>
-        <v>1.6470000000000002</v>
+        <v>1.0980000000000001</v>
       </c>
       <c r="J27" s="13">
         <f t="shared" si="1"/>
-        <v>2.0587500000000003</v>
+        <v>1.3725000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>16</v>
@@ -2214,10 +2229,10 @@
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G28" s="1">
         <v>1</v>
@@ -2236,22 +2251,22 @@
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2270,22 +2285,22 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="G30" s="1">
         <v>1</v>
@@ -2304,22 +2319,22 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G31" s="11">
         <v>1</v>
@@ -2338,22 +2353,22 @@
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G32" s="1">
         <v>1</v>
@@ -2372,22 +2387,22 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G33" s="11">
         <v>1</v>
@@ -2406,22 +2421,22 @@
     </row>
     <row r="34" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="E34" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="G34" s="1">
         <v>1</v>
@@ -2440,22 +2455,22 @@
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="F35" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>106</v>
       </c>
       <c r="G35" s="11">
         <v>1</v>
@@ -2472,24 +2487,24 @@
         <v>3.3000000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
@@ -2508,22 +2523,22 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G37" s="11">
         <v>1</v>
@@ -2542,22 +2557,22 @@
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="E38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="G38" s="1">
         <v>1</v>
@@ -2576,22 +2591,22 @@
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="D39" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="G39" s="11">
         <v>1</v>
@@ -2610,22 +2625,22 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G40" s="1">
         <v>1</v>
@@ -2644,10 +2659,10 @@
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>45</v>
@@ -2656,10 +2671,10 @@
         <v>60</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G41" s="11">
         <v>1</v>
@@ -2678,22 +2693,22 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G42" s="1">
         <v>2</v>
@@ -2712,22 +2727,22 @@
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="D43" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>129</v>
       </c>
       <c r="G43" s="11">
         <v>1</v>
@@ -2746,22 +2761,22 @@
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="17">
+        <v>691243110009</v>
+      </c>
+      <c r="C44" s="17">
+        <v>691243110009</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="17">
+        <v>691243110009</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B44" s="1">
-        <v>691243110009</v>
-      </c>
-      <c r="C44" s="1">
-        <v>691243110009</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E44" s="1">
-        <v>691243110009</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
@@ -2780,22 +2795,22 @@
     </row>
     <row r="45" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B45" s="11">
         <v>61300611821</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E45" s="11">
         <v>61300611821</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G45" s="11">
         <v>1</v>
@@ -2812,333 +2827,345 @@
         <v>0.41875000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A46" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8">
-        <f>SUM(J4:J45)</f>
-        <v>98.037500000000009</v>
+    <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1</v>
+      </c>
+      <c r="H46" s="13">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="I46" s="13">
+        <f t="shared" si="0"/>
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="J46" s="13">
+        <f t="shared" si="1"/>
+        <v>0.74374999999999991</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A47" s="7"/>
+      <c r="A47" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" spans="1:10" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="H48" s="16" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="E49">
-        <v>1</v>
-      </c>
-      <c r="F49" s="9">
+      <c r="I47" s="8"/>
+      <c r="J47" s="8">
+        <f>SUM(J4:J46)</f>
+        <v>98.095000000000013</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="H49" s="16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="9">
         <v>12.62</v>
-      </c>
-      <c r="G49" s="9">
-        <f>F49*E49</f>
-        <v>12.62</v>
-      </c>
-      <c r="H49" s="9">
-        <f>G49*1.25</f>
-        <v>15.774999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="10"/>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" s="9">
-        <v>5.1100000000000003</v>
       </c>
       <c r="G50" s="9">
         <f>F50*E50</f>
+        <v>12.62</v>
+      </c>
+      <c r="H50" s="9">
+        <f>G50*1.25</f>
+        <v>15.774999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="9">
         <v>5.1100000000000003</v>
-      </c>
-      <c r="H50" s="9">
-        <f t="shared" ref="H50:H64" si="2">G50*1.25</f>
-        <v>6.3875000000000002</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" s="9">
-        <v>6.11</v>
       </c>
       <c r="G51" s="9">
         <f>F51*E51</f>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="H51" s="9">
+        <f t="shared" ref="H51:H65" si="2">G51*1.25</f>
+        <v>6.3875000000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="9">
         <v>6.11</v>
       </c>
-      <c r="H51" s="9">
+      <c r="G52" s="9">
+        <f>F52*E52</f>
+        <v>6.11</v>
+      </c>
+      <c r="H52" s="9">
         <f t="shared" si="2"/>
         <v>7.6375000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>217</v>
-      </c>
-      <c r="B52" t="s">
-        <v>216</v>
-      </c>
-      <c r="E52">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>214</v>
+      </c>
+      <c r="B53" t="s">
+        <v>213</v>
+      </c>
+      <c r="E53">
         <v>2</v>
       </c>
-      <c r="F52" s="9">
+      <c r="F53" s="9">
         <v>0.94899999999999995</v>
       </c>
-      <c r="G52" s="9">
-        <f t="shared" ref="G52:G64" si="3">F52*E52</f>
+      <c r="G53" s="9">
+        <f t="shared" ref="G53:G65" si="3">F53*E53</f>
         <v>1.8979999999999999</v>
       </c>
-      <c r="H52" s="9">
+      <c r="H53" s="9">
         <f t="shared" si="2"/>
         <v>2.3725000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>215</v>
       </c>
-      <c r="E53">
+      <c r="B54" t="s">
+        <v>212</v>
+      </c>
+      <c r="E54">
         <v>2</v>
       </c>
-      <c r="F53" s="9">
+      <c r="F54" s="9">
         <v>1.37</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G54" s="9">
         <f t="shared" si="3"/>
         <v>2.74</v>
       </c>
-      <c r="H53" s="9">
+      <c r="H54" s="9">
         <f t="shared" si="2"/>
         <v>3.4250000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>219</v>
-      </c>
-      <c r="B54" t="s">
-        <v>214</v>
-      </c>
-      <c r="E54">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>216</v>
+      </c>
+      <c r="B55" t="s">
+        <v>211</v>
+      </c>
+      <c r="E55">
         <v>2</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F55" s="9">
         <v>0.84</v>
       </c>
-      <c r="G54" s="9">
-        <f t="shared" ref="G54" si="4">F54*E54</f>
+      <c r="G55" s="9">
+        <f t="shared" ref="G55" si="4">F55*E55</f>
         <v>1.68</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H55" s="9">
         <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>147</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-      <c r="F55" s="9">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" s="9">
         <v>0.875</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G56" s="9">
         <f t="shared" si="3"/>
         <v>0.875</v>
       </c>
-      <c r="H55" s="9">
+      <c r="H56" s="9">
         <f t="shared" si="2"/>
         <v>1.09375</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>204</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="E56">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>201</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E57">
         <v>2</v>
       </c>
-      <c r="F56" s="9">
+      <c r="F57" s="9">
         <v>0.85599999999999998</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G57" s="9">
         <f t="shared" si="3"/>
         <v>1.712</v>
       </c>
-      <c r="H56" s="9">
+      <c r="H57" s="9">
         <f t="shared" si="2"/>
         <v>2.14</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57" s="9">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" s="9">
         <v>3.45</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G58" s="9">
         <f t="shared" si="3"/>
         <v>3.45</v>
       </c>
-      <c r="H57" s="9">
+      <c r="H58" s="9">
         <f t="shared" si="2"/>
         <v>4.3125</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>148</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58" s="9">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>145</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" s="9">
         <v>5</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G59" s="9">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="H58" s="9">
+      <c r="H59" s="9">
         <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>209</v>
-      </c>
-      <c r="B59" t="s">
-        <v>208</v>
-      </c>
-      <c r="E59">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>206</v>
+      </c>
+      <c r="B60" t="s">
+        <v>205</v>
+      </c>
+      <c r="E60">
         <v>4</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F60" s="9">
         <v>0.1</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G60" s="9">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="H59" s="9">
+      <c r="H60" s="9">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>210</v>
-      </c>
-      <c r="B60" t="s">
-        <v>211</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60" s="9">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>207</v>
+      </c>
+      <c r="B61" t="s">
+        <v>208</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" s="9">
         <v>0.1</v>
       </c>
-      <c r="G60" s="9">
-        <f t="shared" ref="G60" si="5">F60*E60</f>
+      <c r="G61" s="9">
+        <f t="shared" ref="G61" si="5">F61*E61</f>
         <v>0.1</v>
       </c>
-      <c r="H60" s="9">
+      <c r="H61" s="9">
         <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B61" t="s">
-        <v>150</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61" s="9">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B62" t="s">
+        <v>147</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="9">
         <v>0.2</v>
       </c>
-      <c r="G61" s="9">
-        <f>F59*E59</f>
-        <v>0.4</v>
-      </c>
-      <c r="H61" s="9">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B62" t="s">
-        <v>151</v>
-      </c>
-      <c r="E62">
-        <v>4</v>
-      </c>
-      <c r="F62" s="9">
-        <v>0.1</v>
-      </c>
       <c r="G62" s="9">
-        <f t="shared" si="3"/>
+        <f>F60*E60</f>
         <v>0.4</v>
       </c>
       <c r="H62" s="9">
@@ -3148,266 +3175,288 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>152</v>
+        <v>209</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F63" s="9">
         <v>0.1</v>
       </c>
       <c r="G63" s="9">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H63" s="9">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B64" t="s">
-        <v>232</v>
+        <v>150</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F64" s="9">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G64" s="9">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="H64" s="9">
         <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B65" t="s">
+        <v>229</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" s="9">
+        <v>1</v>
+      </c>
+      <c r="G65" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H65" s="9">
+        <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A65" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8">
-        <f>SUM(H62:H64)+SUM(H58:H60)+SUM(H51:H56)+H49</f>
+    <row r="66" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8">
+        <f>SUM(H63:H65)+SUM(H59:H61)+SUM(H52:H57)+H50</f>
         <v>43.418750000000003</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="17" t="s">
+    <row r="68" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" t="s">
+        <v>203</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" s="9">
+        <v>171.4</v>
+      </c>
+      <c r="G69" s="9">
+        <f t="shared" ref="G69" si="6">F69*E69</f>
+        <v>171.4</v>
+      </c>
+      <c r="H69">
+        <f>G69*1.25</f>
+        <v>214.25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="G71" s="9"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>155</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>156</v>
-      </c>
-      <c r="B68" t="s">
-        <v>206</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68" s="9">
-        <v>171.4</v>
-      </c>
-      <c r="G68" s="9">
-        <f t="shared" ref="G68" si="6">F68*E68</f>
-        <v>171.4</v>
-      </c>
-      <c r="H68">
-        <f>G68*1.25</f>
-        <v>214.25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-    </row>
-    <row r="70" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>158</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="E71">
-        <v>1</v>
-      </c>
-      <c r="F71" s="9">
+      <c r="B72" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" s="9">
         <v>17</v>
       </c>
-      <c r="G71" s="9">
-        <f>F71*E71</f>
+      <c r="G72" s="9">
+        <f>F72*E72</f>
         <v>17</v>
       </c>
-      <c r="H71" s="9">
-        <f>G71*1.25</f>
+      <c r="H72" s="9">
+        <f>G72*1.25</f>
         <v>21.25</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-    </row>
-    <row r="73" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="B73" s="17"/>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F73" s="9"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>160</v>
-      </c>
-      <c r="B74" t="s">
-        <v>235</v>
-      </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="F74" s="9">
-        <v>66.34</v>
-      </c>
-      <c r="G74" s="9">
-        <f t="shared" ref="G74:G75" si="7">F74*E74</f>
-        <v>66.34</v>
-      </c>
-      <c r="H74" s="9">
-        <f t="shared" ref="H74:H79" si="8">G74*1.25</f>
-        <v>82.925000000000011</v>
-      </c>
+    <row r="74" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B74" s="18"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>236</v>
+        <v>157</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E75">
         <v>1</v>
       </c>
       <c r="F75" s="9">
+        <v>66.34</v>
+      </c>
+      <c r="G75" s="9">
+        <f t="shared" ref="G75:G76" si="7">F75*E75</f>
+        <v>66.34</v>
+      </c>
+      <c r="H75" s="9">
+        <f t="shared" ref="H75:H80" si="8">G75*1.25</f>
+        <v>82.925000000000011</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>233</v>
+      </c>
+      <c r="B76" t="s">
+        <v>234</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" s="9">
         <v>38.340000000000003</v>
       </c>
-      <c r="G75" s="9">
+      <c r="G76" s="9">
         <f t="shared" si="7"/>
         <v>38.340000000000003</v>
       </c>
-      <c r="H75" s="9">
+      <c r="H76" s="9">
         <f t="shared" si="8"/>
         <v>47.925000000000004</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A76" s="7"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="17" t="s">
+    <row r="77" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A77" s="7"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="9"/>
+    </row>
+    <row r="78" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="B78" s="18"/>
+      <c r="H78" s="9"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>236</v>
+      </c>
+      <c r="B79" t="s">
         <v>238</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="H77" s="9"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>239</v>
-      </c>
-      <c r="B78" t="s">
-        <v>241</v>
-      </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78" s="9">
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79" s="9">
         <v>18</v>
       </c>
-      <c r="G78" s="9">
-        <f t="shared" ref="G78:G79" si="9">F78*E78</f>
+      <c r="G79" s="9">
+        <f t="shared" ref="G79:G80" si="9">F79*E79</f>
         <v>18</v>
       </c>
-      <c r="H78" s="9">
+      <c r="H79" s="9">
         <f t="shared" si="8"/>
         <v>22.5</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>240</v>
-      </c>
-      <c r="B79" t="s">
-        <v>242</v>
-      </c>
-      <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79" s="9">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80" t="s">
+        <v>239</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" s="9">
         <v>17</v>
       </c>
-      <c r="G79" s="9">
+      <c r="G80" s="9">
         <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="H79" s="9">
+      <c r="H80" s="9">
         <f t="shared" si="8"/>
         <v>21.25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="F77:G77"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C71:D71"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D23" r:id="rId1" display="https://eu.mouser.com/manufacturer/cui-devices/" xr:uid="{20A6F0EA-5529-4B15-9D5D-90A5BC0CFECC}"/>
-    <hyperlink ref="B55" r:id="rId2" xr:uid="{5A33C5A7-DC1C-4D1C-82D4-6F10AD1F10D3}"/>
-    <hyperlink ref="B56" r:id="rId3" xr:uid="{537D6D9C-9F20-4B7C-8ECD-54BA77D8ACC7}"/>
-    <hyperlink ref="B57" r:id="rId4" xr:uid="{DC7B44C9-7248-43F5-9F3E-3B4750BAB0D5}"/>
-    <hyperlink ref="C68" r:id="rId5" xr:uid="{1D7E88CD-AFAA-4B97-9D92-1ED605380133}"/>
-    <hyperlink ref="B71" r:id="rId6" xr:uid="{51F49AE6-72ED-40A6-BE54-4BFB91B32B23}"/>
+    <hyperlink ref="B56" r:id="rId2" xr:uid="{5A33C5A7-DC1C-4D1C-82D4-6F10AD1F10D3}"/>
+    <hyperlink ref="B57" r:id="rId3" xr:uid="{537D6D9C-9F20-4B7C-8ECD-54BA77D8ACC7}"/>
+    <hyperlink ref="B58" r:id="rId4" xr:uid="{DC7B44C9-7248-43F5-9F3E-3B4750BAB0D5}"/>
+    <hyperlink ref="C69" r:id="rId5" xr:uid="{1D7E88CD-AFAA-4B97-9D92-1ED605380133}"/>
+    <hyperlink ref="B72" r:id="rId6" xr:uid="{51F49AE6-72ED-40A6-BE54-4BFB91B32B23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct typo in BOM
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56743B9C-CCD9-4D87-BC59-902D76FE9F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3C3E21-4C76-496D-B35E-700CB96C551B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,9 +471,6 @@
     <t>For enclosure to JBS stand</t>
   </si>
   <si>
-    <t xml:space="preserve">For the binder 99-0624-00-07 </t>
-  </si>
-  <si>
     <t>Screws - M2x8mm + nuts</t>
   </si>
   <si>
@@ -779,6 +776,9 @@
   </si>
   <si>
     <t>200-TSW10807TS</t>
+  </si>
+  <si>
+    <t>To mount HIROSE(HRS) RPC1-12RB-6P(71)</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1313,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M62" sqref="M62"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,13 +1333,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="24"/>
@@ -1353,7 +1353,7 @@
       <c r="A2" s="21"/>
       <c r="B2" s="23"/>
       <c r="C2" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1377,7 +1377,7 @@
         <v>133</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>3</v>
@@ -1386,18 +1386,18 @@
         <v>134</v>
       </c>
       <c r="H3" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>197</v>
-      </c>
       <c r="J3" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="5" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>9</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -1499,22 +1499,22 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>187</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="G7" s="11">
         <v>1</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="8" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>20</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>29</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B13" s="11">
         <v>100</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
@@ -1771,22 +1771,22 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>190</v>
       </c>
       <c r="G15" s="11">
         <v>1</v>
@@ -1805,22 +1805,22 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -1842,7 +1842,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>42</v>
@@ -1851,10 +1851,10 @@
         <v>40</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G17" s="11">
         <v>1</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>58</v>
@@ -2013,7 +2013,7 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>63</v>
@@ -2047,22 +2047,22 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>112</v>
       </c>
       <c r="E23" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="G23" s="11">
         <v>1</v>
@@ -2118,7 +2118,7 @@
         <v>71</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>72</v>
@@ -2127,10 +2127,10 @@
         <v>56</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G25" s="11">
         <v>1</v>
@@ -2183,22 +2183,22 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>77</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G27" s="11">
         <v>2</v>
@@ -2254,19 +2254,19 @@
         <v>82</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>178</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2322,19 +2322,19 @@
         <v>88</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>179</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>180</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G31" s="11">
         <v>1</v>
@@ -2390,19 +2390,19 @@
         <v>94</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G33" s="11">
         <v>1</v>
@@ -2489,7 +2489,7 @@
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>95</v>
@@ -2523,22 +2523,22 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>183</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>184</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E37" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>223</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>224</v>
       </c>
       <c r="G37" s="11">
         <v>1</v>
@@ -2693,7 +2693,7 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>136</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="45" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B45" s="11">
         <v>61300611821</v>
@@ -2829,22 +2829,22 @@
     </row>
     <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="C46" s="17" t="s">
         <v>248</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>249</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G46" s="1">
         <v>1</v>
@@ -2892,12 +2892,12 @@
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="H49" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B50" s="25"/>
       <c r="C50" s="25"/>
@@ -2958,10 +2958,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -2980,10 +2980,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B54" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -3002,10 +3002,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -3027,7 +3027,7 @@
         <v>144</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -3046,10 +3046,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>200</v>
+      </c>
+      <c r="B57" s="15" t="s">
         <v>201</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>202</v>
       </c>
       <c r="E57">
         <v>2</v>
@@ -3068,10 +3068,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -3109,10 +3109,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E60">
         <v>4</v>
@@ -3131,10 +3131,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>206</v>
+      </c>
+      <c r="B61" t="s">
         <v>207</v>
-      </c>
-      <c r="B61" t="s">
-        <v>208</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -3175,10 +3175,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B63" t="s">
-        <v>148</v>
+        <v>250</v>
       </c>
       <c r="E63">
         <v>4</v>
@@ -3197,10 +3197,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B64" t="s">
         <v>149</v>
-      </c>
-      <c r="B64" t="s">
-        <v>150</v>
       </c>
       <c r="E64">
         <v>2</v>
@@ -3219,10 +3219,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B65" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="66" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="68" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
@@ -3264,13 +3264,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B69" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -3293,7 +3293,7 @@
     </row>
     <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B71" s="18"/>
       <c r="C71" s="18"/>
@@ -3302,10 +3302,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="74" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B74" s="18"/>
       <c r="G74" s="9"/>
@@ -3337,10 +3337,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B75" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -3359,10 +3359,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>232</v>
+      </c>
+      <c r="B76" t="s">
         <v>233</v>
-      </c>
-      <c r="B76" t="s">
-        <v>234</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -3387,17 +3387,17 @@
     </row>
     <row r="78" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B78" s="18"/>
       <c r="H78" s="9"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B79" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -3416,10 +3416,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B80" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E80">
         <v>1</v>

</xml_diff>

<commit_message>
Update footprint name of STL9P3LLH6 to be correct
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelj\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel Johansson\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3C3E21-4C76-496D-B35E-700CB96C551B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D306EC-AF42-43FC-A266-6D0FB0F56D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="250">
   <si>
     <t>References</t>
   </si>
@@ -373,9 +373,6 @@
   </si>
   <si>
     <t>STL9P3LLH6</t>
-  </si>
-  <si>
-    <t>STL20N6F7</t>
   </si>
   <si>
     <t>511-STL9P3LLH6</t>
@@ -786,10 +783,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -945,23 +942,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
@@ -974,7 +971,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1313,8 +1310,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,13 +1330,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="24"/>
@@ -1353,7 +1350,7 @@
       <c r="A2" s="21"/>
       <c r="B2" s="23"/>
       <c r="C2" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1374,30 +1371,30 @@
         <v>2</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H3" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>196</v>
-      </c>
       <c r="J3" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1431,7 +1428,7 @@
     </row>
     <row r="5" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>9</v>
@@ -1465,7 +1462,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -1480,7 +1477,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G6" s="1">
         <v>2</v>
@@ -1499,22 +1496,22 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>161</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>162</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>187</v>
       </c>
       <c r="G7" s="11">
         <v>1</v>
@@ -1533,7 +1530,7 @@
     </row>
     <row r="8" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1567,7 +1564,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>20</v>
@@ -1601,7 +1598,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -1635,7 +1632,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>29</v>
@@ -1669,7 +1666,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -1703,7 +1700,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B13" s="11">
         <v>100</v>
@@ -1737,7 +1734,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
@@ -1771,22 +1768,22 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>188</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>189</v>
       </c>
       <c r="G15" s="11">
         <v>1</v>
@@ -1805,22 +1802,22 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -1842,7 +1839,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>42</v>
@@ -1851,10 +1848,10 @@
         <v>40</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G17" s="11">
         <v>1</v>
@@ -1979,7 +1976,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>58</v>
@@ -2013,7 +2010,7 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>63</v>
@@ -2047,22 +2044,22 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>112</v>
       </c>
       <c r="E23" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="G23" s="11">
         <v>1</v>
@@ -2118,7 +2115,7 @@
         <v>71</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>72</v>
@@ -2127,10 +2124,10 @@
         <v>56</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G25" s="11">
         <v>1</v>
@@ -2183,22 +2180,22 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>77</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G27" s="11">
         <v>2</v>
@@ -2254,19 +2251,19 @@
         <v>82</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2322,19 +2319,19 @@
         <v>88</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>179</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G31" s="11">
         <v>1</v>
@@ -2390,19 +2387,19 @@
         <v>94</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G33" s="11">
         <v>1</v>
@@ -2489,7 +2486,7 @@
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>95</v>
@@ -2523,22 +2520,22 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>182</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>183</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E37" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>222</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>223</v>
       </c>
       <c r="G37" s="11">
         <v>1</v>
@@ -2597,7 +2594,7 @@
         <v>115</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>92</v>
@@ -2606,7 +2603,7 @@
         <v>115</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G39" s="11">
         <v>1</v>
@@ -2625,22 +2622,22 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>92</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="G40" s="1">
         <v>1</v>
@@ -2659,10 +2656,10 @@
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>45</v>
@@ -2671,10 +2668,10 @@
         <v>60</v>
       </c>
       <c r="E41" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F41" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>120</v>
       </c>
       <c r="G41" s="11">
         <v>1</v>
@@ -2693,22 +2690,22 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="G42" s="1">
         <v>2</v>
@@ -2727,22 +2724,22 @@
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="C43" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F43" s="11" t="s">
         <v>126</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="G43" s="11">
         <v>1</v>
@@ -2761,7 +2758,7 @@
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B44" s="17">
         <v>691243110009</v>
@@ -2770,13 +2767,13 @@
         <v>691243110009</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E44" s="17">
         <v>691243110009</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G44" s="1">
         <v>1</v>
@@ -2795,22 +2792,22 @@
     </row>
     <row r="45" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B45" s="11">
         <v>61300611821</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E45" s="11">
         <v>61300611821</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G45" s="11">
         <v>1</v>
@@ -2829,22 +2826,22 @@
     </row>
     <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="C46" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="D46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="G46" s="1">
         <v>1</v>
@@ -2863,7 +2860,7 @@
     </row>
     <row r="47" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -2887,17 +2884,17 @@
     </row>
     <row r="49" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="H49" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B50" s="25"/>
       <c r="C50" s="25"/>
@@ -2918,7 +2915,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B51" s="10"/>
       <c r="E51">
@@ -2938,7 +2935,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B52" s="3"/>
       <c r="E52">
@@ -2958,10 +2955,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -2980,10 +2977,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -3002,10 +2999,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B55" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -3024,10 +3021,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -3046,10 +3043,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>199</v>
+      </c>
+      <c r="B57" s="15" t="s">
         <v>200</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>201</v>
       </c>
       <c r="E57">
         <v>2</v>
@@ -3068,10 +3065,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -3090,7 +3087,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -3109,10 +3106,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B60" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E60">
         <v>4</v>
@@ -3131,10 +3128,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B61" t="s">
         <v>206</v>
-      </c>
-      <c r="B61" t="s">
-        <v>207</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -3153,10 +3150,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" t="s">
         <v>146</v>
-      </c>
-      <c r="B62" t="s">
-        <v>147</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -3175,10 +3172,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E63">
         <v>4</v>
@@ -3197,10 +3194,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B64" t="s">
         <v>148</v>
-      </c>
-      <c r="B64" t="s">
-        <v>149</v>
       </c>
       <c r="E64">
         <v>2</v>
@@ -3219,10 +3216,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B65" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -3241,7 +3238,7 @@
     </row>
     <row r="66" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -3256,7 +3253,7 @@
     </row>
     <row r="68" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
@@ -3264,13 +3261,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -3293,7 +3290,7 @@
     </row>
     <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B71" s="18"/>
       <c r="C71" s="18"/>
@@ -3302,10 +3299,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -3329,7 +3326,7 @@
     </row>
     <row r="74" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B74" s="18"/>
       <c r="G74" s="9"/>
@@ -3337,10 +3334,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -3359,10 +3356,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>231</v>
+      </c>
+      <c r="B76" t="s">
         <v>232</v>
-      </c>
-      <c r="B76" t="s">
-        <v>233</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -3387,17 +3384,17 @@
     </row>
     <row r="78" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B78" s="18"/>
       <c r="H78" s="9"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B79" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -3416,10 +3413,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B80" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E80">
         <v>1</v>

</xml_diff>

<commit_message>
update rest alu-plate thickness to 2 mm.
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel Johansson\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D306EC-AF42-43FC-A266-6D0FB0F56D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7B9892-7BD1-4518-907A-E769048957A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15435" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,9 +474,6 @@
     <t>For the aluminium rest</t>
   </si>
   <si>
-    <t>Aluminium plate 15x10x3 mm</t>
-  </si>
-  <si>
     <t>JBC stand</t>
   </si>
   <si>
@@ -776,6 +773,9 @@
   </si>
   <si>
     <t>To mount HIROSE(HRS) RPC1-12RB-6P(71)</t>
+  </si>
+  <si>
+    <t>Aluminium plate 15x10x2 mm</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1310,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,13 +1330,13 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="24"/>
@@ -1350,7 +1350,7 @@
       <c r="A2" s="21"/>
       <c r="B2" s="23"/>
       <c r="C2" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1374,7 +1374,7 @@
         <v>132</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>3</v>
@@ -1383,18 +1383,18 @@
         <v>133</v>
       </c>
       <c r="H3" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="I3" s="16" t="s">
-        <v>195</v>
-      </c>
       <c r="J3" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="5" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>9</v>
@@ -1462,7 +1462,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
@@ -1496,22 +1496,22 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>160</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>161</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="G7" s="11">
         <v>1</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="8" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>20</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>29</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B13" s="11">
         <v>100</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>34</v>
@@ -1768,22 +1768,22 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>187</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="G15" s="11">
         <v>1</v>
@@ -1802,22 +1802,22 @@
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -1839,7 +1839,7 @@
         <v>41</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>42</v>
@@ -1848,10 +1848,10 @@
         <v>40</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G17" s="11">
         <v>1</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>58</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>63</v>
@@ -2044,22 +2044,22 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>112</v>
       </c>
       <c r="E23" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>196</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>197</v>
       </c>
       <c r="G23" s="11">
         <v>1</v>
@@ -2115,7 +2115,7 @@
         <v>71</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>72</v>
@@ -2124,10 +2124,10 @@
         <v>56</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G25" s="11">
         <v>1</v>
@@ -2180,22 +2180,22 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>77</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G27" s="11">
         <v>2</v>
@@ -2251,19 +2251,19 @@
         <v>82</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>176</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2319,19 +2319,19 @@
         <v>88</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>178</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G31" s="11">
         <v>1</v>
@@ -2387,19 +2387,19 @@
         <v>94</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G33" s="11">
         <v>1</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>95</v>
@@ -2520,22 +2520,22 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>181</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>85</v>
       </c>
       <c r="E37" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>221</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>222</v>
       </c>
       <c r="G37" s="11">
         <v>1</v>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>135</v>
@@ -2792,7 +2792,7 @@
     </row>
     <row r="45" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B45" s="11">
         <v>61300611821</v>
@@ -2826,22 +2826,22 @@
     </row>
     <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="C46" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>247</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G46" s="1">
         <v>1</v>
@@ -2889,12 +2889,12 @@
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="H49" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B50" s="25"/>
       <c r="C50" s="25"/>
@@ -2955,10 +2955,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -2977,10 +2977,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -2999,10 +2999,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B55" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -3024,7 +3024,7 @@
         <v>143</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -3043,10 +3043,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>198</v>
+      </c>
+      <c r="B57" s="15" t="s">
         <v>199</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>200</v>
       </c>
       <c r="E57">
         <v>2</v>
@@ -3065,10 +3065,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -3106,10 +3106,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B60" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E60">
         <v>4</v>
@@ -3128,10 +3128,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>204</v>
+      </c>
+      <c r="B61" t="s">
         <v>205</v>
-      </c>
-      <c r="B61" t="s">
-        <v>206</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -3172,10 +3172,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B63" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E63">
         <v>4</v>
@@ -3216,10 +3216,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>149</v>
+        <v>249</v>
       </c>
       <c r="B65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="66" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="68" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
@@ -3261,13 +3261,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B71" s="18"/>
       <c r="C71" s="18"/>
@@ -3299,10 +3299,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -3326,7 +3326,7 @@
     </row>
     <row r="74" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B74" s="18"/>
       <c r="G74" s="9"/>
@@ -3334,10 +3334,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B75" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -3356,10 +3356,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" t="s">
         <v>231</v>
-      </c>
-      <c r="B76" t="s">
-        <v>232</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -3384,17 +3384,17 @@
     </row>
     <row r="78" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B78" s="18"/>
       <c r="H78" s="9"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B79" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -3413,10 +3413,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B80" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E80">
         <v>1</v>

</xml_diff>

<commit_message>
Update schematic and BOM for hw 3.2
</commit_message>
<xml_diff>
--- a/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
+++ b/AxxSolder_hardware/bom/BOM_AxxSolder_V3_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axel Johansson\ownCloud\2_Project\00_AxxProjects\AxxSolder\AxxSolder_hardware\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7B9892-7BD1-4518-907A-E769048957A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D15EB-E14F-4425-B457-83219F0BB8EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15435" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{60354D9D-8798-4211-B1E3-D5485177CC9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="253">
   <si>
     <t>References</t>
   </si>
@@ -754,9 +754,6 @@
     <t>S2, S3</t>
   </si>
   <si>
-    <t>AxxSolder V3.1</t>
-  </si>
-  <si>
     <t>TFT1</t>
   </si>
   <si>
@@ -776,6 +773,18 @@
   </si>
   <si>
     <t>Aluminium plate 15x10x2 mm</t>
+  </si>
+  <si>
+    <t>R49,R50</t>
+  </si>
+  <si>
+    <t>ERJ-3RED10R0V</t>
+  </si>
+  <si>
+    <t>667-ERJ-3RED10R0V</t>
+  </si>
+  <si>
+    <t>AxxSolder V3.2</t>
   </si>
 </sst>
 </file>
@@ -1308,10 +1317,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3ACC24B-AB82-4A13-8EC7-565525F2C562}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1339,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>207</v>
@@ -1452,11 +1461,11 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="I5" s="13">
-        <f t="shared" ref="I5:I46" si="0">G5*H5</f>
+        <f t="shared" ref="I5:I47" si="0">G5*H5</f>
         <v>2.8319999999999999</v>
       </c>
       <c r="J5" s="13">
-        <f t="shared" ref="J5:J46" si="1">1.25*I5</f>
+        <f t="shared" ref="J5:J47" si="1">1.25*I5</f>
         <v>3.54</v>
       </c>
     </row>
@@ -1835,1356 +1844,1368 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0.121</v>
+      </c>
+      <c r="I17" s="13">
+        <f t="shared" si="0"/>
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="J17" s="13">
+        <f t="shared" si="1"/>
+        <v>0.30249999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="G17" s="11">
-        <v>1</v>
-      </c>
-      <c r="H17" s="14">
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
+      <c r="H18" s="14">
         <v>0.753</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I18" s="13">
         <f t="shared" si="0"/>
         <v>0.753</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J18" s="13">
         <f t="shared" si="1"/>
         <v>0.94125000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G19" s="1">
         <v>4</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H19" s="13">
         <v>0.112</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I19" s="13">
         <f t="shared" si="0"/>
         <v>0.44800000000000001</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J19" s="13">
         <f t="shared" si="1"/>
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G20" s="11">
         <v>2</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H20" s="14">
         <v>0.19500000000000001</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I20" s="13">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J20" s="13">
         <f t="shared" si="1"/>
         <v>0.48750000000000004</v>
-      </c>
-      <c r="K19" s="12"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="1">
-        <v>2</v>
-      </c>
-      <c r="H20" s="13">
-        <v>0.4</v>
-      </c>
-      <c r="I20" s="13">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="J20" s="13">
-        <f t="shared" si="1"/>
-        <v>1</v>
       </c>
       <c r="K20" s="12"/>
       <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="I21" s="13">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="J21" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K21" s="12"/>
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="11">
+      <c r="G22" s="11">
         <v>2</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H22" s="14">
         <v>0.372</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I22" s="13">
         <f t="shared" si="0"/>
         <v>0.74399999999999999</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J22" s="13">
         <f t="shared" si="1"/>
         <v>0.92999999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4311</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="13">
+        <v>18.55</v>
+      </c>
+      <c r="I23" s="13">
+        <f t="shared" si="0"/>
+        <v>18.55</v>
+      </c>
+      <c r="J23" s="13">
+        <f t="shared" si="1"/>
+        <v>23.1875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G24" s="11">
+        <v>1</v>
+      </c>
+      <c r="H24" s="14">
+        <v>2.37</v>
+      </c>
+      <c r="I24" s="13">
+        <f t="shared" si="0"/>
+        <v>2.37</v>
+      </c>
+      <c r="J24" s="13">
+        <f t="shared" si="1"/>
+        <v>2.9625000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="13">
+        <v>1.6</v>
+      </c>
+      <c r="I25" s="13">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="J25" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="G26" s="11">
+        <v>1</v>
+      </c>
+      <c r="H26" s="14">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="I26" s="13">
+        <f t="shared" si="0"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="J26" s="13">
+        <f t="shared" si="1"/>
+        <v>3.1875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="I27" s="13">
+        <f t="shared" si="0"/>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="J27" s="13">
+        <f t="shared" si="1"/>
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="G28" s="11">
+        <v>2</v>
+      </c>
+      <c r="H28" s="14">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I28" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="J28" s="13">
+        <f t="shared" si="1"/>
+        <v>1.3725000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="13">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="I29" s="13">
+        <f t="shared" si="0"/>
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="J29" s="13">
+        <f t="shared" si="1"/>
+        <v>0.22125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="G30" s="11">
+        <v>1</v>
+      </c>
+      <c r="H30" s="14">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="I30" s="13">
+        <f t="shared" si="0"/>
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="J30" s="13">
+        <f t="shared" si="1"/>
+        <v>0.47625000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="13">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I31" s="13">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J31" s="13">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="G32" s="11">
+        <v>1</v>
+      </c>
+      <c r="H32" s="14">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="I32" s="13">
+        <f t="shared" si="0"/>
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="J32" s="13">
+        <f t="shared" si="1"/>
+        <v>1.20875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="13">
+        <v>5.65</v>
+      </c>
+      <c r="I33" s="13">
+        <f t="shared" si="0"/>
+        <v>5.65</v>
+      </c>
+      <c r="J33" s="13">
+        <f t="shared" si="1"/>
+        <v>7.0625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="G34" s="11">
+        <v>1</v>
+      </c>
+      <c r="H34" s="14">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="I34" s="13">
+        <f t="shared" si="0"/>
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="J34" s="13">
+        <f t="shared" si="1"/>
+        <v>0.40750000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="13">
+        <v>2.52</v>
+      </c>
+      <c r="I35" s="13">
+        <f t="shared" si="0"/>
+        <v>2.52</v>
+      </c>
+      <c r="J35" s="13">
+        <f t="shared" si="1"/>
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G36" s="11">
+        <v>1</v>
+      </c>
+      <c r="H36" s="14">
+        <v>2.64</v>
+      </c>
+      <c r="I36" s="13">
+        <f t="shared" si="0"/>
+        <v>2.64</v>
+      </c>
+      <c r="J36" s="13">
+        <f t="shared" si="1"/>
+        <v>3.3000000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="13">
+        <v>5.22</v>
+      </c>
+      <c r="I37" s="13">
+        <f t="shared" si="0"/>
+        <v>5.22</v>
+      </c>
+      <c r="J37" s="13">
+        <f t="shared" si="1"/>
+        <v>6.5249999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="G38" s="11">
+        <v>1</v>
+      </c>
+      <c r="H38" s="14">
+        <v>2.74</v>
+      </c>
+      <c r="I38" s="13">
+        <f t="shared" si="0"/>
+        <v>2.74</v>
+      </c>
+      <c r="J38" s="13">
+        <f t="shared" si="1"/>
+        <v>3.4250000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="13">
+        <v>2.71</v>
+      </c>
+      <c r="I39" s="13">
+        <f t="shared" si="0"/>
+        <v>2.71</v>
+      </c>
+      <c r="J39" s="13">
+        <f t="shared" si="1"/>
+        <v>3.3875000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G40" s="11">
+        <v>1</v>
+      </c>
+      <c r="H40" s="14">
+        <v>0.995</v>
+      </c>
+      <c r="I40" s="13">
+        <f t="shared" si="0"/>
+        <v>0.995</v>
+      </c>
+      <c r="J40" s="13">
+        <f t="shared" si="1"/>
+        <v>1.2437499999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
+      <c r="H41" s="13">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="I41" s="13">
+        <f t="shared" si="0"/>
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="J41" s="13">
+        <f t="shared" si="1"/>
+        <v>1.20875</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" s="11">
+        <v>1</v>
+      </c>
+      <c r="H42" s="14">
+        <v>0.13</v>
+      </c>
+      <c r="I42" s="13">
+        <f t="shared" si="0"/>
+        <v>0.13</v>
+      </c>
+      <c r="J42" s="13">
+        <f t="shared" si="1"/>
+        <v>0.16250000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2</v>
+      </c>
+      <c r="H43" s="13">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="I43" s="13">
+        <f t="shared" si="0"/>
+        <v>0.186</v>
+      </c>
+      <c r="J43" s="13">
+        <f t="shared" si="1"/>
+        <v>0.23249999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G44" s="11">
+        <v>1</v>
+      </c>
+      <c r="H44" s="14">
+        <v>1.26</v>
+      </c>
+      <c r="I44" s="13">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+      <c r="J44" s="13">
+        <f t="shared" si="1"/>
+        <v>1.575</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="17">
+        <v>691243110009</v>
+      </c>
+      <c r="C45" s="17">
+        <v>691243110009</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="17">
+        <v>691243110009</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+      <c r="H45" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="I45" s="13">
+        <f t="shared" si="0"/>
+        <v>3.7</v>
+      </c>
+      <c r="J45" s="13">
+        <f t="shared" si="1"/>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="11">
+        <v>61300611821</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="11">
+        <v>61300611821</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" s="11">
+        <v>1</v>
+      </c>
+      <c r="H46" s="14">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="I46" s="13">
+        <f t="shared" si="0"/>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="J46" s="13">
+        <f t="shared" si="1"/>
+        <v>0.41875000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="1">
-        <v>4311</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" s="1">
-        <v>1</v>
-      </c>
-      <c r="H22" s="13">
-        <v>18.55</v>
-      </c>
-      <c r="I22" s="13">
-        <f t="shared" si="0"/>
-        <v>18.55</v>
-      </c>
-      <c r="J22" s="13">
-        <f t="shared" si="1"/>
-        <v>23.1875</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="G23" s="11">
-        <v>1</v>
-      </c>
-      <c r="H23" s="14">
-        <v>2.37</v>
-      </c>
-      <c r="I23" s="13">
-        <f t="shared" si="0"/>
-        <v>2.37</v>
-      </c>
-      <c r="J23" s="13">
-        <f t="shared" si="1"/>
-        <v>2.9625000000000004</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="13">
-        <v>1.6</v>
-      </c>
-      <c r="I24" s="13">
-        <f t="shared" si="0"/>
-        <v>1.6</v>
-      </c>
-      <c r="J24" s="13">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="G25" s="11">
-        <v>1</v>
-      </c>
-      <c r="H25" s="14">
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="I25" s="13">
-        <f t="shared" si="0"/>
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="J25" s="13">
-        <f t="shared" si="1"/>
-        <v>3.1875</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" s="1">
-        <v>1</v>
-      </c>
-      <c r="H26" s="13">
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="I26" s="13">
-        <f t="shared" si="0"/>
-        <v>0.72499999999999998</v>
-      </c>
-      <c r="J26" s="13">
-        <f t="shared" si="1"/>
-        <v>0.90625</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="G27" s="11">
-        <v>2</v>
-      </c>
-      <c r="H27" s="14">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="I27" s="13">
-        <f t="shared" si="0"/>
-        <v>1.0980000000000001</v>
-      </c>
-      <c r="J27" s="13">
-        <f t="shared" si="1"/>
-        <v>1.3725000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G28" s="1">
-        <v>1</v>
-      </c>
-      <c r="H28" s="13">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="I28" s="13">
-        <f t="shared" si="0"/>
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="J28" s="13">
-        <f t="shared" si="1"/>
-        <v>0.22125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="G29" s="11">
-        <v>1</v>
-      </c>
-      <c r="H29" s="14">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="I29" s="13">
-        <f t="shared" si="0"/>
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="J29" s="13">
-        <f t="shared" si="1"/>
-        <v>0.47625000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" s="1">
-        <v>1</v>
-      </c>
-      <c r="H30" s="13">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I30" s="13">
-        <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J30" s="13">
-        <f t="shared" si="1"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="G31" s="11">
-        <v>1</v>
-      </c>
-      <c r="H31" s="14">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="I31" s="13">
-        <f t="shared" si="0"/>
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="J31" s="13">
-        <f t="shared" si="1"/>
-        <v>1.20875</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" s="13">
-        <v>5.65</v>
-      </c>
-      <c r="I32" s="13">
-        <f t="shared" si="0"/>
-        <v>5.65</v>
-      </c>
-      <c r="J32" s="13">
-        <f t="shared" si="1"/>
-        <v>7.0625</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G33" s="11">
-        <v>1</v>
-      </c>
-      <c r="H33" s="14">
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="I33" s="13">
-        <f t="shared" si="0"/>
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="J33" s="13">
-        <f t="shared" si="1"/>
-        <v>0.40750000000000003</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G34" s="1">
-        <v>1</v>
-      </c>
-      <c r="H34" s="13">
-        <v>2.52</v>
-      </c>
-      <c r="I34" s="13">
-        <f t="shared" si="0"/>
-        <v>2.52</v>
-      </c>
-      <c r="J34" s="13">
-        <f t="shared" si="1"/>
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G35" s="11">
-        <v>1</v>
-      </c>
-      <c r="H35" s="14">
-        <v>2.64</v>
-      </c>
-      <c r="I35" s="13">
-        <f t="shared" si="0"/>
-        <v>2.64</v>
-      </c>
-      <c r="J35" s="13">
-        <f t="shared" si="1"/>
-        <v>3.3000000000000003</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G36" s="1">
-        <v>1</v>
-      </c>
-      <c r="H36" s="13">
-        <v>5.22</v>
-      </c>
-      <c r="I36" s="13">
-        <f t="shared" si="0"/>
-        <v>5.22</v>
-      </c>
-      <c r="J36" s="13">
-        <f t="shared" si="1"/>
-        <v>6.5249999999999995</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="G37" s="11">
-        <v>1</v>
-      </c>
-      <c r="H37" s="14">
-        <v>2.74</v>
-      </c>
-      <c r="I37" s="13">
-        <f t="shared" si="0"/>
-        <v>2.74</v>
-      </c>
-      <c r="J37" s="13">
-        <f t="shared" si="1"/>
-        <v>3.4250000000000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1</v>
-      </c>
-      <c r="H38" s="13">
-        <v>2.71</v>
-      </c>
-      <c r="I38" s="13">
-        <f t="shared" si="0"/>
-        <v>2.71</v>
-      </c>
-      <c r="J38" s="13">
-        <f t="shared" si="1"/>
-        <v>3.3875000000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G39" s="11">
-        <v>1</v>
-      </c>
-      <c r="H39" s="14">
-        <v>0.995</v>
-      </c>
-      <c r="I39" s="13">
-        <f t="shared" si="0"/>
-        <v>0.995</v>
-      </c>
-      <c r="J39" s="13">
-        <f t="shared" si="1"/>
-        <v>1.2437499999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1</v>
-      </c>
-      <c r="H40" s="13">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="I40" s="13">
-        <f t="shared" si="0"/>
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="J40" s="13">
-        <f t="shared" si="1"/>
-        <v>1.20875</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="G41" s="11">
-        <v>1</v>
-      </c>
-      <c r="H41" s="14">
-        <v>0.13</v>
-      </c>
-      <c r="I41" s="13">
-        <f t="shared" si="0"/>
-        <v>0.13</v>
-      </c>
-      <c r="J41" s="13">
-        <f t="shared" si="1"/>
-        <v>0.16250000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="B47" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G42" s="1">
-        <v>2</v>
-      </c>
-      <c r="H42" s="13">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="I42" s="13">
-        <f t="shared" si="0"/>
-        <v>0.186</v>
-      </c>
-      <c r="J42" s="13">
-        <f t="shared" si="1"/>
-        <v>0.23249999999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G43" s="11">
-        <v>1</v>
-      </c>
-      <c r="H43" s="14">
-        <v>1.26</v>
-      </c>
-      <c r="I43" s="13">
-        <f t="shared" si="0"/>
-        <v>1.26</v>
-      </c>
-      <c r="J43" s="13">
-        <f t="shared" si="1"/>
-        <v>1.575</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B44" s="17">
-        <v>691243110009</v>
-      </c>
-      <c r="C44" s="17">
-        <v>691243110009</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="17">
-        <v>691243110009</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="13">
-        <v>3.7</v>
-      </c>
-      <c r="I44" s="13">
-        <f t="shared" si="0"/>
-        <v>3.7</v>
-      </c>
-      <c r="J44" s="13">
-        <f t="shared" si="1"/>
-        <v>4.625</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B45" s="11">
-        <v>61300611821</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" s="11">
-        <v>61300611821</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="G45" s="11">
-        <v>1</v>
-      </c>
-      <c r="H45" s="14">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="I45" s="13">
-        <f t="shared" si="0"/>
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="J45" s="13">
-        <f t="shared" si="1"/>
-        <v>0.41875000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="E47" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="B46" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="C46" s="17" t="s">
+      <c r="F47" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="G46" s="1">
-        <v>1</v>
-      </c>
-      <c r="H46" s="13">
+      <c r="G47" s="1">
+        <v>1</v>
+      </c>
+      <c r="H47" s="13">
         <v>0.59499999999999997</v>
       </c>
-      <c r="I46" s="13">
+      <c r="I47" s="13">
         <f t="shared" si="0"/>
         <v>0.59499999999999997</v>
       </c>
-      <c r="J46" s="13">
+      <c r="J47" s="13">
         <f t="shared" si="1"/>
         <v>0.74374999999999991</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A47" s="7" t="s">
+    <row r="48" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8">
-        <f>SUM(J4:J46)</f>
-        <v>98.095000000000013</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="5" t="s">
+      <c r="I48" s="8"/>
+      <c r="J48" s="8">
+        <f>SUM(J4:J47)</f>
+        <v>98.397500000000022</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="H49" s="16" t="s">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="H50" s="16" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" s="9">
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" s="9">
         <v>12.62</v>
-      </c>
-      <c r="G50" s="9">
-        <f>F50*E50</f>
-        <v>12.62</v>
-      </c>
-      <c r="H50" s="9">
-        <f>G50*1.25</f>
-        <v>15.774999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B51" s="10"/>
-      <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51" s="9">
-        <v>5.1100000000000003</v>
       </c>
       <c r="G51" s="9">
         <f>F51*E51</f>
+        <v>12.62</v>
+      </c>
+      <c r="H51" s="9">
+        <f>G51*1.25</f>
+        <v>15.774999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" s="9">
         <v>5.1100000000000003</v>
-      </c>
-      <c r="H51" s="9">
-        <f t="shared" ref="H51:H65" si="2">G51*1.25</f>
-        <v>6.3875000000000002</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="E52">
-        <v>1</v>
-      </c>
-      <c r="F52" s="9">
-        <v>6.11</v>
       </c>
       <c r="G52" s="9">
         <f>F52*E52</f>
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="H52" s="9">
+        <f t="shared" ref="H52:H66" si="2">G52*1.25</f>
+        <v>6.3875000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" s="9">
         <v>6.11</v>
       </c>
-      <c r="H52" s="9">
+      <c r="G53" s="9">
+        <f>F53*E53</f>
+        <v>6.11</v>
+      </c>
+      <c r="H53" s="9">
         <f t="shared" si="2"/>
         <v>7.6375000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>211</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>210</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>2</v>
       </c>
-      <c r="F53" s="9">
+      <c r="F54" s="9">
         <v>0.94899999999999995</v>
       </c>
-      <c r="G53" s="9">
-        <f t="shared" ref="G53:G65" si="3">F53*E53</f>
+      <c r="G54" s="9">
+        <f t="shared" ref="G54:G66" si="3">F54*E54</f>
         <v>1.8979999999999999</v>
       </c>
-      <c r="H53" s="9">
+      <c r="H54" s="9">
         <f t="shared" si="2"/>
         <v>2.3725000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>212</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>209</v>
       </c>
-      <c r="E54">
+      <c r="E55">
         <v>2</v>
       </c>
-      <c r="F54" s="9">
+      <c r="F55" s="9">
         <v>1.37</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G55" s="9">
         <f t="shared" si="3"/>
         <v>2.74</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H55" s="9">
         <f t="shared" si="2"/>
         <v>3.4250000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>213</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>208</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <v>2</v>
       </c>
-      <c r="F55" s="9">
+      <c r="F56" s="9">
         <v>0.84</v>
       </c>
-      <c r="G55" s="9">
-        <f t="shared" ref="G55" si="4">F55*E55</f>
+      <c r="G56" s="9">
+        <f t="shared" ref="G56" si="4">F56*E56</f>
         <v>1.68</v>
       </c>
-      <c r="H55" s="9">
+      <c r="H56" s="9">
         <f t="shared" si="2"/>
         <v>2.1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>143</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B57" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-      <c r="F56" s="9">
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" s="9">
         <v>0.875</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G57" s="9">
         <f t="shared" si="3"/>
         <v>0.875</v>
       </c>
-      <c r="H56" s="9">
+      <c r="H57" s="9">
         <f t="shared" si="2"/>
         <v>1.09375</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>198</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B58" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="E57">
+      <c r="E58">
         <v>2</v>
       </c>
-      <c r="F57" s="9">
+      <c r="F58" s="9">
         <v>0.85599999999999998</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G58" s="9">
         <f t="shared" si="3"/>
         <v>1.712</v>
       </c>
-      <c r="H57" s="9">
+      <c r="H58" s="9">
         <f t="shared" si="2"/>
         <v>2.14</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B59" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58" s="9">
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" s="9">
         <v>3.45</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G59" s="9">
         <f t="shared" si="3"/>
         <v>3.45</v>
       </c>
-      <c r="H58" s="9">
+      <c r="H59" s="9">
         <f t="shared" si="2"/>
         <v>4.3125</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>144</v>
       </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59" s="9">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" s="9">
         <v>5</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G60" s="9">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="H59" s="9">
+      <c r="H60" s="9">
         <f t="shared" si="2"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>203</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>202</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <v>4</v>
       </c>
-      <c r="F60" s="9">
+      <c r="F61" s="9">
         <v>0.1</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G61" s="9">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
-      <c r="H60" s="9">
+      <c r="H61" s="9">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>204</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>205</v>
       </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61" s="9">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" s="9">
         <v>0.1</v>
       </c>
-      <c r="G61" s="9">
-        <f t="shared" ref="G61" si="5">F61*E61</f>
+      <c r="G62" s="9">
+        <f t="shared" ref="G62" si="5">F62*E62</f>
         <v>0.1</v>
       </c>
-      <c r="H61" s="9">
+      <c r="H62" s="9">
         <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>146</v>
       </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62" s="9">
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="9">
         <v>0.2</v>
       </c>
-      <c r="G62" s="9">
-        <f>F60*E60</f>
-        <v>0.4</v>
-      </c>
-      <c r="H62" s="9">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B63" t="s">
-        <v>248</v>
-      </c>
-      <c r="E63">
-        <v>4</v>
-      </c>
-      <c r="F63" s="9">
-        <v>0.1</v>
-      </c>
       <c r="G63" s="9">
-        <f t="shared" si="3"/>
+        <f>F61*E61</f>
         <v>0.4</v>
       </c>
       <c r="H63" s="9">
@@ -3194,266 +3215,288 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="B64" t="s">
-        <v>148</v>
+        <v>247</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F64" s="9">
         <v>0.1</v>
       </c>
       <c r="G64" s="9">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H64" s="9">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>249</v>
+        <v>147</v>
       </c>
       <c r="B65" t="s">
-        <v>226</v>
+        <v>148</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F65" s="9">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G65" s="9">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="H65" s="9">
         <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B66" t="s">
+        <v>226</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="9">
+        <v>1</v>
+      </c>
+      <c r="G66" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="H66" s="9">
+        <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A66" s="7" t="s">
+    <row r="67" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A67" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8">
-        <f>SUM(H63:H65)+SUM(H59:H61)+SUM(H52:H57)+H50</f>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8">
+        <f>SUM(H64:H66)+SUM(H60:H62)+SUM(H53:H58)+H51</f>
         <v>43.418750000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="18" t="s">
+    <row r="69" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>150</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>200</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C70" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="E69">
-        <v>1</v>
-      </c>
-      <c r="F69" s="9">
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" s="9">
         <v>171.4</v>
       </c>
-      <c r="G69" s="9">
-        <f t="shared" ref="G69" si="6">F69*E69</f>
+      <c r="G70" s="9">
+        <f t="shared" ref="G70" si="6">F70*E70</f>
         <v>171.4</v>
       </c>
-      <c r="H69">
-        <f>G69*1.25</f>
+      <c r="H70">
+        <f>G70*1.25</f>
         <v>214.25</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F70" s="9"/>
-      <c r="G70" s="9"/>
-    </row>
-    <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="18" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+    </row>
+    <row r="72" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="G71" s="9"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="G72" s="9"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>152</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B73" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="E72">
-        <v>1</v>
-      </c>
-      <c r="F72" s="9">
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" s="9">
         <v>17</v>
       </c>
-      <c r="G72" s="9">
-        <f>F72*E72</f>
+      <c r="G73" s="9">
+        <f>F73*E73</f>
         <v>17</v>
       </c>
-      <c r="H72" s="9">
-        <f>G72*1.25</f>
+      <c r="H73" s="9">
+        <f>G73*1.25</f>
         <v>21.25</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-    </row>
-    <row r="74" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="B74" s="18"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>154</v>
-      </c>
-      <c r="B75" t="s">
-        <v>229</v>
-      </c>
-      <c r="E75">
-        <v>1</v>
-      </c>
-      <c r="F75" s="9">
-        <v>66.34</v>
-      </c>
-      <c r="G75" s="9">
-        <f t="shared" ref="G75:G76" si="7">F75*E75</f>
-        <v>66.34</v>
-      </c>
-      <c r="H75" s="9">
-        <f t="shared" ref="H75:H80" si="8">G75*1.25</f>
-        <v>82.925000000000011</v>
-      </c>
+    <row r="75" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75" s="18"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" t="s">
+        <v>229</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" s="9">
+        <v>66.34</v>
+      </c>
+      <c r="G76" s="9">
+        <f t="shared" ref="G76:G77" si="7">F76*E76</f>
+        <v>66.34</v>
+      </c>
+      <c r="H76" s="9">
+        <f t="shared" ref="H76:H81" si="8">G76*1.25</f>
+        <v>82.925000000000011</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>230</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>231</v>
       </c>
-      <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="F76" s="9">
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" s="9">
         <v>38.340000000000003</v>
       </c>
-      <c r="G76" s="9">
+      <c r="G77" s="9">
         <f t="shared" si="7"/>
         <v>38.340000000000003</v>
       </c>
-      <c r="H76" s="9">
+      <c r="H77" s="9">
         <f t="shared" si="8"/>
         <v>47.925000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A77" s="7"/>
-      <c r="F77" s="19"/>
-      <c r="G77" s="19"/>
-      <c r="H77" s="9"/>
-    </row>
-    <row r="78" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" s="18" t="s">
+    <row r="78" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A78" s="7"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="9"/>
+    </row>
+    <row r="79" spans="1:8" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="H78" s="9"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="B79" s="18"/>
+      <c r="H79" s="9"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>233</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>235</v>
       </c>
-      <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79" s="9">
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" s="9">
         <v>18</v>
       </c>
-      <c r="G79" s="9">
-        <f t="shared" ref="G79:G80" si="9">F79*E79</f>
+      <c r="G80" s="9">
+        <f t="shared" ref="G80:G81" si="9">F80*E80</f>
         <v>18</v>
       </c>
-      <c r="H79" s="9">
+      <c r="H80" s="9">
         <f t="shared" si="8"/>
         <v>22.5</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>234</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>236</v>
       </c>
-      <c r="E80">
-        <v>1</v>
-      </c>
-      <c r="F80" s="9">
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81" s="9">
         <v>17</v>
       </c>
-      <c r="G80" s="9">
+      <c r="G81" s="9">
         <f t="shared" si="9"/>
         <v>17</v>
       </c>
-      <c r="H80" s="9">
+      <c r="H81" s="9">
         <f t="shared" si="8"/>
         <v>21.25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="F78:G78"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C72:D72"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D23" r:id="rId1" display="https://eu.mouser.com/manufacturer/cui-devices/" xr:uid="{20A6F0EA-5529-4B15-9D5D-90A5BC0CFECC}"/>
-    <hyperlink ref="B56" r:id="rId2" xr:uid="{5A33C5A7-DC1C-4D1C-82D4-6F10AD1F10D3}"/>
-    <hyperlink ref="B57" r:id="rId3" xr:uid="{537D6D9C-9F20-4B7C-8ECD-54BA77D8ACC7}"/>
-    <hyperlink ref="B58" r:id="rId4" xr:uid="{DC7B44C9-7248-43F5-9F3E-3B4750BAB0D5}"/>
-    <hyperlink ref="C69" r:id="rId5" xr:uid="{1D7E88CD-AFAA-4B97-9D92-1ED605380133}"/>
-    <hyperlink ref="B72" r:id="rId6" xr:uid="{51F49AE6-72ED-40A6-BE54-4BFB91B32B23}"/>
+    <hyperlink ref="D24" r:id="rId1" display="https://eu.mouser.com/manufacturer/cui-devices/" xr:uid="{20A6F0EA-5529-4B15-9D5D-90A5BC0CFECC}"/>
+    <hyperlink ref="B57" r:id="rId2" xr:uid="{5A33C5A7-DC1C-4D1C-82D4-6F10AD1F10D3}"/>
+    <hyperlink ref="B58" r:id="rId3" xr:uid="{537D6D9C-9F20-4B7C-8ECD-54BA77D8ACC7}"/>
+    <hyperlink ref="B59" r:id="rId4" xr:uid="{DC7B44C9-7248-43F5-9F3E-3B4750BAB0D5}"/>
+    <hyperlink ref="C70" r:id="rId5" xr:uid="{1D7E88CD-AFAA-4B97-9D92-1ED605380133}"/>
+    <hyperlink ref="B73" r:id="rId6" xr:uid="{51F49AE6-72ED-40A6-BE54-4BFB91B32B23}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>